<commit_message>
update predict.py and color npm dataset
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="semantic3d" sheetId="1" r:id="rId1"/>
     <sheet name="npm3d" sheetId="2" r:id="rId2"/>
-    <sheet name="semantic2npm" sheetId="3" r:id="rId3"/>
+    <sheet name="common_class" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
   <si>
     <t>model_name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -101,10 +101,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>s</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>use_geometry</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -177,6 +173,30 @@
   </si>
   <si>
     <t>cars</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ours</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>semantic_cross_npm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>semantic2npm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dataset_transfer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>npm2npm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pointsemantic</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -512,15 +532,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S16"/>
+  <dimension ref="A1:S10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.25" customWidth="1"/>
+    <col min="1" max="1" width="19.625" customWidth="1"/>
     <col min="2" max="2" width="11.875" customWidth="1"/>
     <col min="3" max="3" width="10.625" customWidth="1"/>
     <col min="4" max="4" width="11.875" customWidth="1"/>
@@ -529,7 +549,7 @@
     <col min="7" max="7" width="10.25" customWidth="1"/>
     <col min="8" max="8" width="10.5" customWidth="1"/>
     <col min="11" max="11" width="6.75" customWidth="1"/>
-    <col min="12" max="12" width="18" customWidth="1"/>
+    <col min="12" max="12" width="12.625" customWidth="1"/>
     <col min="13" max="13" width="13.25" customWidth="1"/>
     <col min="14" max="14" width="14.375" customWidth="1"/>
     <col min="15" max="15" width="13.125" customWidth="1"/>
@@ -549,13 +569,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -594,7 +614,7 @@
         <v>15</v>
       </c>
       <c r="S1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
@@ -953,7 +973,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8">
         <v>8192</v>
@@ -1012,7 +1032,7 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9">
         <v>8192</v>
@@ -1035,10 +1055,97 @@
       <c r="H9">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="I16" t="s">
-        <v>21</v>
+      <c r="I9">
+        <v>40</v>
+      </c>
+      <c r="J9">
+        <v>0.65811299999999995</v>
+      </c>
+      <c r="K9">
+        <v>0.89662500000000001</v>
+      </c>
+      <c r="L9">
+        <v>0.90305599999999997</v>
+      </c>
+      <c r="M9">
+        <v>0.69113800000000003</v>
+      </c>
+      <c r="N9">
+        <v>0.895814</v>
+      </c>
+      <c r="O9">
+        <v>0.37152800000000002</v>
+      </c>
+      <c r="P9">
+        <v>0.91305499999999995</v>
+      </c>
+      <c r="Q9">
+        <v>0.316799</v>
+      </c>
+      <c r="R9">
+        <v>0.55424600000000002</v>
+      </c>
+      <c r="S9">
+        <v>0.61926800000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10">
+        <v>8192</v>
+      </c>
+      <c r="C10">
+        <v>16</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>10</v>
+      </c>
+      <c r="H10">
+        <v>10</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>0.13391500000000001</v>
+      </c>
+      <c r="K10">
+        <v>0.44855600000000001</v>
+      </c>
+      <c r="L10">
+        <v>0.38561000000000001</v>
+      </c>
+      <c r="M10">
+        <v>0.237426</v>
+      </c>
+      <c r="N10">
+        <v>2.8600000000000001E-4</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0.43162800000000001</v>
+      </c>
+      <c r="Q10">
+        <v>1.6371E-2</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1050,10 +1157,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection sqref="A1:T2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1079,13 +1186,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -1103,36 +1210,36 @@
         <v>8</v>
       </c>
       <c r="L1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" t="s">
         <v>25</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>26</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>27</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>28</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>30</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>31</v>
       </c>
-      <c r="S1" t="s">
-        <v>32</v>
-      </c>
       <c r="T1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2">
         <v>8192</v>
@@ -1190,6 +1297,68 @@
       </c>
       <c r="T2">
         <v>0.68004799999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3">
+        <v>8192</v>
+      </c>
+      <c r="C3">
+        <v>16</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>10</v>
+      </c>
+      <c r="I3">
+        <v>50</v>
+      </c>
+      <c r="J3">
+        <v>0.66985799999999995</v>
+      </c>
+      <c r="K3">
+        <v>0.962615</v>
+      </c>
+      <c r="L3">
+        <v>0.97357199999999999</v>
+      </c>
+      <c r="M3">
+        <v>0.95247999999999999</v>
+      </c>
+      <c r="N3">
+        <v>0.64186900000000002</v>
+      </c>
+      <c r="O3">
+        <v>0.59559300000000004</v>
+      </c>
+      <c r="P3">
+        <v>0.40692699999999998</v>
+      </c>
+      <c r="Q3">
+        <v>0.40978100000000001</v>
+      </c>
+      <c r="R3">
+        <v>0.39611200000000002</v>
+      </c>
+      <c r="S3">
+        <v>0.84192199999999995</v>
+      </c>
+      <c r="T3">
+        <v>0.81046499999999999</v>
       </c>
     </row>
   </sheetData>
@@ -1201,74 +1370,113 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.125" customWidth="1"/>
-    <col min="2" max="2" width="9.875" customWidth="1"/>
+    <col min="2" max="2" width="15.25" customWidth="1"/>
+    <col min="3" max="3" width="9.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>36</v>
       </c>
-      <c r="B1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2">
         <v>7</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>0.73899999999999999</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>0.93569999999999998</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>0.92789999999999995</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0.61229999999999996</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>0.9365</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>0.35670000000000002</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>0.86170000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>0.83209999999999995</v>
+      </c>
+      <c r="E3">
+        <v>0.96519999999999995</v>
+      </c>
+      <c r="F3">
+        <v>0.97370000000000001</v>
+      </c>
+      <c r="G3">
+        <v>0.81569999999999998</v>
+      </c>
+      <c r="H3">
+        <v>0.95469999999999999</v>
+      </c>
+      <c r="I3">
+        <v>0.52929999999999999</v>
+      </c>
+      <c r="J3">
+        <v>0.88680000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
normalize geometry before feeding to network
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
   <si>
     <t>model_name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -119,100 +119,111 @@
     <t>building</t>
   </si>
   <si>
+    <t>cars and trunks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>row</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>model_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pointnet2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ground</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nature</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>building</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hardscape</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cars</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ours</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>semantic_cross_npm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>semantic2npm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dataset_transfer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>npm2npm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pointsemantic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pointcnn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pointsemantic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[0:1]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[1:2]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[2:3]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>pole - road sign - traffic light</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>bollard - small pole</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>trash can</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>barrier</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>pedestrian</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>car</t>
-  </si>
-  <si>
-    <t>cars and trunks</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>natural - vegetation</t>
-  </si>
-  <si>
-    <t>row</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>model_name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pointnet2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ground</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nature</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>building</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>hardscape</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cars</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ours</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>semantic_cross_npm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>semantic2npm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dataset_transfer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>npm2npm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pointsemantic</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pointcnn</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pointsemantic</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[0:1]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[1:2]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -548,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S13"/>
+  <dimension ref="A1:S14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -630,7 +641,7 @@
         <v>15</v>
       </c>
       <c r="S1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
@@ -1107,7 +1118,7 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B10">
         <v>8192</v>
@@ -1166,7 +1177,7 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B11">
         <v>8192</v>
@@ -1225,7 +1236,7 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B12">
         <v>8192</v>
@@ -1240,7 +1251,7 @@
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="G12">
         <v>10</v>
@@ -1284,7 +1295,7 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B13">
         <v>8192</v>
@@ -1299,13 +1310,105 @@
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="G13">
         <v>10</v>
       </c>
       <c r="H13">
         <v>10</v>
+      </c>
+      <c r="I13">
+        <v>40</v>
+      </c>
+      <c r="J13">
+        <v>0.63315699999999997</v>
+      </c>
+      <c r="K13">
+        <v>0.88558999999999999</v>
+      </c>
+      <c r="L13">
+        <v>0.87949500000000003</v>
+      </c>
+      <c r="M13">
+        <v>0.65441899999999997</v>
+      </c>
+      <c r="N13">
+        <v>0.88510999999999995</v>
+      </c>
+      <c r="O13">
+        <v>0.37359900000000001</v>
+      </c>
+      <c r="P13">
+        <v>0.89678000000000002</v>
+      </c>
+      <c r="Q13">
+        <v>0.30763000000000001</v>
+      </c>
+      <c r="R13">
+        <v>0.534501</v>
+      </c>
+      <c r="S13">
+        <v>0.53371900000000005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14">
+        <v>8192</v>
+      </c>
+      <c r="C14">
+        <v>16</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14">
+        <v>10</v>
+      </c>
+      <c r="H14">
+        <v>10</v>
+      </c>
+      <c r="I14">
+        <v>15</v>
+      </c>
+      <c r="J14">
+        <v>0.487541</v>
+      </c>
+      <c r="K14">
+        <v>0.813558</v>
+      </c>
+      <c r="L14">
+        <v>0.82316500000000004</v>
+      </c>
+      <c r="M14">
+        <v>0.61223399999999994</v>
+      </c>
+      <c r="N14">
+        <v>0.80680600000000002</v>
+      </c>
+      <c r="O14">
+        <v>0.23685800000000001</v>
+      </c>
+      <c r="P14">
+        <v>0.74796099999999999</v>
+      </c>
+      <c r="Q14">
+        <v>0.143812</v>
+      </c>
+      <c r="R14">
+        <v>0.24742400000000001</v>
+      </c>
+      <c r="S14">
+        <v>0.28206599999999998</v>
       </c>
     </row>
   </sheetData>
@@ -1319,8 +1422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1376,25 +1479,25 @@
         <v>25</v>
       </c>
       <c r="N1" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="O1" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="P1" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="Q1" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="R1" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="S1" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="T1" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
@@ -1461,7 +1564,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B3">
         <v>8192</v>
@@ -1533,7 +1636,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1545,13 +1648,13 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
         <v>6</v>
@@ -1560,27 +1663,27 @@
         <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="G1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="H1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="I1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="J1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -1609,10 +1712,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C3">
         <v>2</v>

</xml_diff>

<commit_message>
generate normals by open3d
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="74">
   <si>
     <t>model_name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -159,10 +159,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>semantic_cross_npm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>semantic2npm</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -256,6 +252,62 @@
   </si>
   <si>
     <t>npm2semantic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>npm2semantic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pointcnn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>npm2semantic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pointnet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>semantic2npm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pointnet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[4:5]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pointsemantic_cross</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pointsemantic_cross</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pointsemantic_cross</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>semantic2npm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>normals</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>normals(open3d)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>normals(open3d)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -316,10 +368,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -600,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S16"/>
+  <dimension ref="A1:T19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -612,21 +665,21 @@
     <col min="2" max="2" width="11.875" customWidth="1"/>
     <col min="3" max="3" width="10.625" customWidth="1"/>
     <col min="4" max="4" width="11.875" customWidth="1"/>
-    <col min="5" max="5" width="11.625" customWidth="1"/>
-    <col min="6" max="6" width="13.25" customWidth="1"/>
-    <col min="7" max="7" width="10.25" customWidth="1"/>
-    <col min="8" max="8" width="10.5" customWidth="1"/>
-    <col min="11" max="11" width="9.25" customWidth="1"/>
-    <col min="12" max="12" width="12.625" customWidth="1"/>
-    <col min="13" max="13" width="13.25" customWidth="1"/>
-    <col min="14" max="14" width="14.375" customWidth="1"/>
-    <col min="15" max="15" width="13.125" customWidth="1"/>
-    <col min="17" max="17" width="10.25" customWidth="1"/>
-    <col min="18" max="18" width="15" customWidth="1"/>
-    <col min="19" max="19" width="13.125" customWidth="1"/>
+    <col min="5" max="6" width="11.625" customWidth="1"/>
+    <col min="7" max="7" width="13.25" customWidth="1"/>
+    <col min="8" max="8" width="10.25" customWidth="1"/>
+    <col min="9" max="9" width="10.5" customWidth="1"/>
+    <col min="12" max="12" width="9.25" customWidth="1"/>
+    <col min="13" max="13" width="12.625" customWidth="1"/>
+    <col min="14" max="14" width="13.25" customWidth="1"/>
+    <col min="15" max="15" width="14.375" customWidth="1"/>
+    <col min="16" max="16" width="13.125" customWidth="1"/>
+    <col min="18" max="18" width="10.25" customWidth="1"/>
+    <col min="19" max="19" width="15" customWidth="1"/>
+    <col min="20" max="20" width="13.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -640,52 +693,55 @@
         <v>23</v>
       </c>
       <c r="E1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
-        <v>10</v>
-      </c>
       <c r="N1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>15</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -699,52 +755,55 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H2">
         <v>10</v>
       </c>
       <c r="I2">
+        <v>10</v>
+      </c>
+      <c r="J2">
         <v>95</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>0.65688000000000002</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>0.905385</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>0.91800499999999996</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>0.78905199999999998</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>0.90249900000000005</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>0.32696799999999998</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>0.91301200000000005</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>0.278281</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>0.51377899999999999</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>0.61344100000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -764,46 +823,49 @@
         <v>0</v>
       </c>
       <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
         <v>60</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>20</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>70</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>0.186386</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>0.50136800000000004</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>0.345472</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>0.195965</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>0.37651299999999999</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>5.0841999999999998E-2</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>0.44557099999999999</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>5.5694E-2</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>6.182E-3</v>
       </c>
-      <c r="S3">
+      <c r="T3">
         <v>1.4848999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -823,47 +885,50 @@
         <v>0</v>
       </c>
       <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
         <v>60</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>20</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>65</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>0.45910200000000001</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>0.80827499999999997</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>0.72771200000000003</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>0.33360099999999998</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>0.80377299999999996</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>0.21134500000000001</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>0.80785200000000001</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>0.180178</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>0.31795800000000002</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <v>0.29039799999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B5">
@@ -882,46 +947,49 @@
         <v>0</v>
       </c>
       <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
         <v>60</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>20</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>85</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>0.188746</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>0.47884700000000002</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>0.398285</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>0.18503700000000001</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>0.28633799999999998</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>5.7312000000000002E-2</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>0.42391200000000001</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>7.3982000000000006E-2</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>2.6446000000000001E-2</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <v>5.8653999999999998E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
@@ -935,52 +1003,55 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <v>10</v>
       </c>
       <c r="I6">
+        <v>10</v>
+      </c>
+      <c r="J6">
         <v>120</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>0.693303</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>0.91327999999999998</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>0.91905700000000001</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>0.75808200000000003</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>0.90187700000000004</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>0.42679400000000001</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>0.91237299999999999</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>0.33857799999999999</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>0.60303499999999999</v>
       </c>
-      <c r="S6">
+      <c r="T6">
         <v>0.68662500000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1000,46 +1071,49 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H7">
         <v>10</v>
       </c>
       <c r="I7">
+        <v>10</v>
+      </c>
+      <c r="J7">
         <v>65</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>0.60308899999999999</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>0.86319500000000005</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>0.760243</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>0.21701500000000001</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>0.88975899999999997</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>0.38575199999999998</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>0.91076800000000002</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>0.33136900000000002</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <v>0.60202699999999998</v>
       </c>
-      <c r="S7">
+      <c r="T7">
         <v>0.72778299999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1053,52 +1127,55 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8" t="s">
-        <v>50</v>
-      </c>
-      <c r="G8">
-        <v>10</v>
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>49</v>
       </c>
       <c r="H8">
         <v>10</v>
       </c>
       <c r="I8">
+        <v>10</v>
+      </c>
+      <c r="J8">
         <v>100</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>0.67700199999999999</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>0.90188000000000001</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>0.90199799999999997</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>0.71543100000000004</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>0.90394300000000005</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>0.367786</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <v>0.99078999999999995</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>0.30444399999999999</v>
       </c>
-      <c r="R8">
+      <c r="S8">
         <v>0.61025600000000002</v>
       </c>
-      <c r="S8">
+      <c r="T8">
         <v>0.71137099999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1112,54 +1189,57 @@
         <v>1</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H9">
         <v>10</v>
       </c>
       <c r="I9">
+        <v>10</v>
+      </c>
+      <c r="J9">
         <v>40</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>0.65811299999999995</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>0.89662500000000001</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>0.90305599999999997</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>0.69113800000000003</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>0.895814</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>0.37152800000000002</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>0.91305499999999995</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>0.316799</v>
       </c>
-      <c r="R9">
+      <c r="S9">
         <v>0.55424600000000002</v>
       </c>
-      <c r="S9">
+      <c r="T9">
         <v>0.61926800000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="B10">
         <v>8192</v>
@@ -1177,48 +1257,51 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H10">
         <v>10</v>
       </c>
       <c r="I10">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
         <v>0.13391500000000001</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>0.44855600000000001</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>0.38561000000000001</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>0.237426</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>2.8600000000000001E-4</v>
       </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
       <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
         <v>0.43162800000000001</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>1.6371E-2</v>
       </c>
-      <c r="R10">
-        <v>0</v>
-      </c>
       <c r="S10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>41</v>
+      <c r="T10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="B11">
         <v>8192</v>
@@ -1230,54 +1313,57 @@
         <v>1</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H11">
         <v>10</v>
       </c>
       <c r="I11">
+        <v>10</v>
+      </c>
+      <c r="J11">
         <v>15</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>0.53214099999999998</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>0.835314</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>0.85293699999999995</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>0.67058200000000001</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <v>0.82112099999999999</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>0.287161</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <v>0.82713400000000004</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <v>0.175315</v>
       </c>
-      <c r="R11">
+      <c r="S11">
         <v>0.27208599999999999</v>
       </c>
-      <c r="S11">
+      <c r="T11">
         <v>0.350796</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12">
         <v>8192</v>
@@ -1289,54 +1375,57 @@
         <v>1</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H12">
         <v>10</v>
       </c>
       <c r="I12">
+        <v>10</v>
+      </c>
+      <c r="J12">
         <v>30</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>0.631552</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>0.87404099999999996</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>0.86173999999999995</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>0.63285599999999997</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <v>0.86813600000000002</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>0.35758299999999998</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
         <v>0.88729999999999998</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>0.26675500000000002</v>
       </c>
-      <c r="R12">
+      <c r="S12">
         <v>0.58054700000000004</v>
       </c>
-      <c r="S12">
+      <c r="T12">
         <v>0.59606599999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B13">
         <v>8192</v>
@@ -1348,54 +1437,57 @@
         <v>1</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H13">
         <v>10</v>
       </c>
       <c r="I13">
+        <v>10</v>
+      </c>
+      <c r="J13">
         <v>40</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>0.63315699999999997</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>0.88558999999999999</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>0.87949500000000003</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>0.65441899999999997</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <v>0.88510999999999995</v>
       </c>
-      <c r="O13">
+      <c r="P13">
         <v>0.37359900000000001</v>
       </c>
-      <c r="P13">
+      <c r="Q13">
         <v>0.89678000000000002</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
         <v>0.30763000000000001</v>
       </c>
-      <c r="R13">
+      <c r="S13">
         <v>0.534501</v>
       </c>
-      <c r="S13">
+      <c r="T13">
         <v>0.53371900000000005</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B14">
         <v>8192</v>
@@ -1407,54 +1499,57 @@
         <v>1</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H14">
         <v>10</v>
       </c>
       <c r="I14">
+        <v>10</v>
+      </c>
+      <c r="J14">
         <v>15</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>0.487541</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>0.813558</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>0.82316500000000004</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>0.61223399999999994</v>
       </c>
-      <c r="N14">
+      <c r="O14">
         <v>0.80680600000000002</v>
       </c>
-      <c r="O14">
+      <c r="P14">
         <v>0.23685800000000001</v>
       </c>
-      <c r="P14">
+      <c r="Q14">
         <v>0.74796099999999999</v>
       </c>
-      <c r="Q14">
+      <c r="R14">
         <v>0.143812</v>
       </c>
-      <c r="R14">
+      <c r="S14">
         <v>0.24742400000000001</v>
       </c>
-      <c r="S14">
+      <c r="T14">
         <v>0.28206599999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15">
         <v>8192</v>
@@ -1466,54 +1561,57 @@
         <v>1</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H15">
         <v>10</v>
       </c>
       <c r="I15">
+        <v>10</v>
+      </c>
+      <c r="J15">
         <v>80</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>0.70425700000000002</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>0.91945600000000005</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>0.91024799999999995</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <v>0.75811300000000004</v>
       </c>
-      <c r="N15">
+      <c r="O15">
         <v>0.91746300000000003</v>
       </c>
-      <c r="O15">
+      <c r="P15">
         <v>0.47132200000000002</v>
       </c>
-      <c r="P15">
+      <c r="Q15">
         <v>0.92657500000000004</v>
       </c>
-      <c r="Q15">
+      <c r="R15">
         <v>0.36943399999999998</v>
       </c>
-      <c r="R15">
+      <c r="S15">
         <v>0.58405399999999996</v>
       </c>
-      <c r="S15">
+      <c r="T15">
         <v>0.69584999999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B16">
         <v>8192</v>
@@ -1525,49 +1623,238 @@
         <v>1</v>
       </c>
       <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16" t="s">
-        <v>56</v>
-      </c>
-      <c r="G16">
-        <v>10</v>
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>55</v>
       </c>
       <c r="H16">
         <v>10</v>
       </c>
       <c r="I16">
+        <v>10</v>
+      </c>
+      <c r="J16">
         <v>30</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>0.62404899999999996</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>0.89718500000000001</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <v>0.89884799999999998</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <v>0.73322900000000002</v>
       </c>
-      <c r="N16">
+      <c r="O16">
         <v>0.89286799999999999</v>
       </c>
-      <c r="O16">
+      <c r="P16">
         <v>0.26639299999999999</v>
       </c>
-      <c r="P16">
+      <c r="Q16">
         <v>0.90962799999999999</v>
       </c>
-      <c r="Q16">
+      <c r="R16">
         <v>0.28854000000000002</v>
       </c>
-      <c r="R16">
+      <c r="S16">
         <v>0.397318</v>
       </c>
-      <c r="S16">
+      <c r="T16">
         <v>0.605568</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17">
+        <v>8192</v>
+      </c>
+      <c r="C17">
+        <v>32</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>10</v>
+      </c>
+      <c r="I17">
+        <v>10</v>
+      </c>
+      <c r="J17">
+        <v>50</v>
+      </c>
+      <c r="K17">
+        <v>0.30713800000000002</v>
+      </c>
+      <c r="L17">
+        <v>0.71615300000000004</v>
+      </c>
+      <c r="M17">
+        <v>0.57201900000000006</v>
+      </c>
+      <c r="N17">
+        <v>0.23003599999999999</v>
+      </c>
+      <c r="O17">
+        <v>0.71056799999999998</v>
+      </c>
+      <c r="P17">
+        <v>6.0545000000000002E-2</v>
+      </c>
+      <c r="Q17">
+        <v>0.66976000000000002</v>
+      </c>
+      <c r="R17">
+        <v>0.12377199999999999</v>
+      </c>
+      <c r="S17">
+        <v>5.7396000000000003E-2</v>
+      </c>
+      <c r="T17">
+        <v>3.3006000000000001E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18">
+        <v>8192</v>
+      </c>
+      <c r="C18">
+        <v>8</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>10</v>
+      </c>
+      <c r="I18">
+        <v>10</v>
+      </c>
+      <c r="J18">
+        <v>15</v>
+      </c>
+      <c r="K18">
+        <v>0.536659</v>
+      </c>
+      <c r="L18">
+        <v>0.84270100000000003</v>
+      </c>
+      <c r="M18">
+        <v>0.75837500000000002</v>
+      </c>
+      <c r="N18">
+        <v>0.296788</v>
+      </c>
+      <c r="O18">
+        <v>0.86892800000000003</v>
+      </c>
+      <c r="P18">
+        <v>0.33066899999999999</v>
+      </c>
+      <c r="Q18">
+        <v>0.87168100000000004</v>
+      </c>
+      <c r="R18">
+        <v>0.23149800000000001</v>
+      </c>
+      <c r="S18">
+        <v>0.51868300000000001</v>
+      </c>
+      <c r="T18">
+        <v>0.41664600000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19">
+        <v>4096</v>
+      </c>
+      <c r="C19">
+        <v>10</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>10</v>
+      </c>
+      <c r="I19">
+        <v>10</v>
+      </c>
+      <c r="J19">
+        <v>40</v>
+      </c>
+      <c r="K19">
+        <v>0.57253200000000004</v>
+      </c>
+      <c r="L19">
+        <v>0.86396799999999996</v>
+      </c>
+      <c r="M19">
+        <v>0.74604999999999999</v>
+      </c>
+      <c r="N19">
+        <v>0.13700300000000001</v>
+      </c>
+      <c r="O19">
+        <v>0.910501</v>
+      </c>
+      <c r="P19">
+        <v>0.40592699999999998</v>
+      </c>
+      <c r="Q19">
+        <v>0.90645500000000001</v>
+      </c>
+      <c r="R19">
+        <v>0.32715</v>
+      </c>
+      <c r="S19">
+        <v>0.50626700000000002</v>
+      </c>
+      <c r="T19">
+        <v>0.64090199999999997</v>
       </c>
     </row>
   </sheetData>
@@ -1579,10 +1866,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U8"/>
+  <dimension ref="A1:U13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1594,7 +1881,7 @@
     <col min="7" max="7" width="14" customWidth="1"/>
     <col min="8" max="8" width="10.125" customWidth="1"/>
     <col min="9" max="9" width="10.375" customWidth="1"/>
-    <col min="21" max="21" width="17.5" customWidth="1"/>
+    <col min="21" max="21" width="10.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
@@ -1611,7 +1898,7 @@
         <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -1641,25 +1928,25 @@
         <v>25</v>
       </c>
       <c r="O1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P1" t="s">
         <v>43</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>44</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>45</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>46</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>47</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>48</v>
-      </c>
-      <c r="U1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
@@ -1728,7 +2015,7 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B3">
@@ -1794,7 +2081,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4">
         <v>8192</v>
@@ -1859,7 +2146,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5">
         <v>8192</v>
@@ -1924,7 +2211,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6">
         <v>8192</v>
@@ -1989,7 +2276,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7">
         <v>8192</v>
@@ -2007,7 +2294,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H7">
         <v>10</v>
@@ -2054,7 +2341,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8">
         <v>8192</v>
@@ -2065,19 +2352,344 @@
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="E8">
-        <v>1</v>
+      <c r="E8" s="3">
+        <v>1E-4</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H8">
         <v>10</v>
       </c>
       <c r="I8">
+        <v>10</v>
+      </c>
+      <c r="J8">
+        <v>50</v>
+      </c>
+      <c r="K8">
+        <v>0.53769299999999998</v>
+      </c>
+      <c r="L8">
+        <v>0.93581700000000001</v>
+      </c>
+      <c r="M8">
+        <v>0.97481499999999999</v>
+      </c>
+      <c r="N8">
+        <v>0.89474699999999996</v>
+      </c>
+      <c r="O8">
+        <v>0.53948300000000005</v>
+      </c>
+      <c r="P8">
+        <v>0.29349799999999998</v>
+      </c>
+      <c r="Q8">
+        <v>0.19156100000000001</v>
+      </c>
+      <c r="R8">
+        <v>0.27735599999999999</v>
+      </c>
+      <c r="S8">
+        <v>0.171344</v>
+      </c>
+      <c r="T8">
+        <v>0.82967299999999999</v>
+      </c>
+      <c r="U8">
+        <v>0.66676199999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9">
+        <v>8192</v>
+      </c>
+      <c r="C9">
+        <v>16</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>66</v>
+      </c>
+      <c r="H9">
+        <v>10</v>
+      </c>
+      <c r="I9">
+        <v>10</v>
+      </c>
+      <c r="J9">
+        <v>70</v>
+      </c>
+      <c r="K9">
+        <v>0.64438700000000004</v>
+      </c>
+      <c r="L9">
+        <v>0.96204999999999996</v>
+      </c>
+      <c r="M9">
+        <v>0.97571799999999997</v>
+      </c>
+      <c r="N9">
+        <v>0.94649000000000005</v>
+      </c>
+      <c r="O9">
+        <v>0.63122599999999995</v>
+      </c>
+      <c r="P9">
+        <v>0.61514599999999997</v>
+      </c>
+      <c r="Q9">
+        <v>0.39865</v>
+      </c>
+      <c r="R9">
+        <v>0.46490799999999999</v>
+      </c>
+      <c r="S9">
+        <v>0.15206900000000001</v>
+      </c>
+      <c r="T9">
+        <v>0.79536799999999996</v>
+      </c>
+      <c r="U9">
+        <v>0.81990700000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <v>8192</v>
+      </c>
+      <c r="C10">
+        <v>16</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>71</v>
+      </c>
+      <c r="H10">
+        <v>10</v>
+      </c>
+      <c r="I10">
+        <v>10</v>
+      </c>
+      <c r="J10">
+        <v>70</v>
+      </c>
+      <c r="K10">
+        <v>0.63486299999999996</v>
+      </c>
+      <c r="L10">
+        <v>0.95802600000000004</v>
+      </c>
+      <c r="M10">
+        <v>0.97563500000000003</v>
+      </c>
+      <c r="N10">
+        <v>0.94070100000000001</v>
+      </c>
+      <c r="O10">
+        <v>0.60836999999999997</v>
+      </c>
+      <c r="P10">
+        <v>0.52667299999999995</v>
+      </c>
+      <c r="Q10">
+        <v>0.39107799999999998</v>
+      </c>
+      <c r="R10">
+        <v>0.46453699999999998</v>
+      </c>
+      <c r="S10">
+        <v>0.166601</v>
+      </c>
+      <c r="T10">
+        <v>0.85980299999999998</v>
+      </c>
+      <c r="U10">
+        <v>0.780366</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11">
+        <v>8192</v>
+      </c>
+      <c r="C11">
+        <v>16</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>71</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="I11">
+        <v>10</v>
+      </c>
+      <c r="J11">
+        <v>30</v>
+      </c>
+      <c r="K11">
+        <v>0.57659800000000005</v>
+      </c>
+      <c r="L11">
+        <v>0.94504699999999997</v>
+      </c>
+      <c r="M11">
+        <v>0.975275</v>
+      </c>
+      <c r="N11">
+        <v>0.91515199999999997</v>
+      </c>
+      <c r="O11">
+        <v>0.61779799999999996</v>
+      </c>
+      <c r="P11">
+        <v>0.44628299999999999</v>
+      </c>
+      <c r="Q11">
+        <v>0.25716800000000001</v>
+      </c>
+      <c r="R11">
+        <v>0.29215799999999997</v>
+      </c>
+      <c r="S11">
+        <v>7.8219999999999998E-2</v>
+      </c>
+      <c r="T11">
+        <v>0.85024900000000003</v>
+      </c>
+      <c r="U11">
+        <v>0.75707899999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12">
+        <v>8192</v>
+      </c>
+      <c r="C12">
+        <v>16</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>72</v>
+      </c>
+      <c r="H12">
+        <v>10</v>
+      </c>
+      <c r="I12">
+        <v>10</v>
+      </c>
+      <c r="J12">
+        <v>15</v>
+      </c>
+      <c r="K12">
+        <v>0.65159900000000004</v>
+      </c>
+      <c r="L12">
+        <v>0.96399800000000002</v>
+      </c>
+      <c r="M12">
+        <v>0.97543299999999999</v>
+      </c>
+      <c r="N12">
+        <v>0.94390399999999997</v>
+      </c>
+      <c r="O12">
+        <v>0.564608</v>
+      </c>
+      <c r="P12">
+        <v>0.42175200000000002</v>
+      </c>
+      <c r="Q12">
+        <v>0.51283199999999995</v>
+      </c>
+      <c r="R12">
+        <v>0.43334099999999998</v>
+      </c>
+      <c r="S12">
+        <v>0.22370200000000001</v>
+      </c>
+      <c r="T12">
+        <v>0.93452500000000005</v>
+      </c>
+      <c r="U12">
+        <v>0.85429299999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>8192</v>
+      </c>
+      <c r="C13">
+        <v>16</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13" t="s">
+        <v>73</v>
+      </c>
+      <c r="H13">
+        <v>10</v>
+      </c>
+      <c r="I13">
         <v>10</v>
       </c>
     </row>
@@ -2090,10 +2702,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2108,7 +2720,7 @@
         <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
         <v>27</v>
@@ -2140,7 +2752,7 @@
         <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -2169,13 +2781,13 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3">
         <v>0.83209999999999995</v>
@@ -2201,10 +2813,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" t="s">
         <v>59</v>
-      </c>
-      <c r="B4" t="s">
-        <v>60</v>
       </c>
       <c r="C4">
         <v>6</v>
@@ -2229,6 +2841,166 @@
       </c>
       <c r="J4">
         <v>0.244743605075426</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>0.62711931710122304</v>
+      </c>
+      <c r="E5">
+        <v>0.86366395672254703</v>
+      </c>
+      <c r="F5">
+        <v>0.756015090024443</v>
+      </c>
+      <c r="G5">
+        <v>0.74500661668205503</v>
+      </c>
+      <c r="H5">
+        <v>0.83539359322613604</v>
+      </c>
+      <c r="I5">
+        <v>0.202195249395108</v>
+      </c>
+      <c r="J5">
+        <v>0.59698603622286694</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>0.45916740651947702</v>
+      </c>
+      <c r="E6">
+        <v>0.65958598521069101</v>
+      </c>
+      <c r="F6">
+        <v>0.68519245979034904</v>
+      </c>
+      <c r="G6">
+        <v>0.61149879068498403</v>
+      </c>
+      <c r="H6">
+        <v>0.40895081138147099</v>
+      </c>
+      <c r="I6">
+        <v>6.5707490893133103E-2</v>
+      </c>
+      <c r="J6">
+        <v>0.52448747984744903</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>0.34809727350436498</v>
+      </c>
+      <c r="E7">
+        <v>0.73025601028565101</v>
+      </c>
+      <c r="F7">
+        <v>0.75223874955741898</v>
+      </c>
+      <c r="G7">
+        <v>0.18502687481340499</v>
+      </c>
+      <c r="H7">
+        <v>0.67744115564151897</v>
+      </c>
+      <c r="I7">
+        <v>0.117655559947803</v>
+      </c>
+      <c r="J7">
+        <v>8.1240275616803696E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8">
+        <v>18</v>
+      </c>
+      <c r="D8">
+        <v>0.585364727359177</v>
+      </c>
+      <c r="E8">
+        <v>0.87157427970707602</v>
+      </c>
+      <c r="F8">
+        <v>0.84744572404534102</v>
+      </c>
+      <c r="G8">
+        <v>0.44379034139513102</v>
+      </c>
+      <c r="H8">
+        <v>0.89542514180549604</v>
+      </c>
+      <c r="I8">
+        <v>0.24798915341724001</v>
+      </c>
+      <c r="J8">
+        <v>0.49217327613267697</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9">
+        <v>19</v>
+      </c>
+      <c r="D9">
+        <v>0.68472463554519702</v>
+      </c>
+      <c r="E9">
+        <v>0.91889793839422995</v>
+      </c>
+      <c r="F9">
+        <v>0.89224273517905595</v>
+      </c>
+      <c r="G9">
+        <v>0.48863351386548498</v>
+      </c>
+      <c r="H9">
+        <v>0.93988980880465101</v>
+      </c>
+      <c r="I9">
+        <v>0.32070629298839898</v>
+      </c>
+      <c r="J9">
+        <v>0.78215082688839299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
save best model by mIoU
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="79">
   <si>
     <t>model_name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -308,6 +308,26 @@
   </si>
   <si>
     <t>normals(open3d)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pointsemantic_cross</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pointsemantic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>semantic2npm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>normals(v3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[0:7](v3)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -653,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T19"/>
+  <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1857,6 +1877,130 @@
         <v>0.64090199999999997</v>
       </c>
     </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20">
+        <v>8192</v>
+      </c>
+      <c r="C20">
+        <v>16</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>10</v>
+      </c>
+      <c r="I20">
+        <v>10</v>
+      </c>
+      <c r="J20">
+        <v>55</v>
+      </c>
+      <c r="K20">
+        <v>0.56194599999999995</v>
+      </c>
+      <c r="L20">
+        <v>0.86346599999999996</v>
+      </c>
+      <c r="M20">
+        <v>0.76452799999999999</v>
+      </c>
+      <c r="N20">
+        <v>0.27819700000000003</v>
+      </c>
+      <c r="O20">
+        <v>0.91461999999999999</v>
+      </c>
+      <c r="P20">
+        <v>0.378002</v>
+      </c>
+      <c r="Q20">
+        <v>0.89576299999999998</v>
+      </c>
+      <c r="R20">
+        <v>0.29931799999999997</v>
+      </c>
+      <c r="S20">
+        <v>0.50759600000000005</v>
+      </c>
+      <c r="T20">
+        <v>0.45754299999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21">
+        <v>4096</v>
+      </c>
+      <c r="C21">
+        <v>16</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>10</v>
+      </c>
+      <c r="I21">
+        <v>10</v>
+      </c>
+      <c r="J21">
+        <v>70</v>
+      </c>
+      <c r="K21">
+        <v>0.556623348955952</v>
+      </c>
+      <c r="L21">
+        <v>0.85663731892903605</v>
+      </c>
+      <c r="M21">
+        <v>0.81200145785372502</v>
+      </c>
+      <c r="N21">
+        <v>0.12601468882875899</v>
+      </c>
+      <c r="O21">
+        <v>0.84036868075598103</v>
+      </c>
+      <c r="P21">
+        <v>0.163312649704833</v>
+      </c>
+      <c r="Q21">
+        <v>0.91681408161611799</v>
+      </c>
+      <c r="R21">
+        <v>0.37705691934178498</v>
+      </c>
+      <c r="S21">
+        <v>0.58968985750209502</v>
+      </c>
+      <c r="T21">
+        <v>0.62772845604432204</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1866,10 +2010,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U13"/>
+  <dimension ref="A1:U15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2015,7 +2159,7 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B3">
@@ -2080,7 +2224,7 @@
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B4">
@@ -2145,7 +2289,7 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B5">
@@ -2210,7 +2354,7 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B6">
@@ -2690,6 +2834,136 @@
         <v>10</v>
       </c>
       <c r="I13">
+        <v>10</v>
+      </c>
+      <c r="J13">
+        <v>40</v>
+      </c>
+      <c r="K13">
+        <v>0.68436200000000003</v>
+      </c>
+      <c r="L13">
+        <v>0.96797500000000003</v>
+      </c>
+      <c r="M13">
+        <v>0.97668699999999997</v>
+      </c>
+      <c r="N13">
+        <v>0.956013</v>
+      </c>
+      <c r="O13">
+        <v>0.67958700000000005</v>
+      </c>
+      <c r="P13">
+        <v>0.51082499999999997</v>
+      </c>
+      <c r="Q13">
+        <v>0.46125500000000003</v>
+      </c>
+      <c r="R13">
+        <v>0.49596299999999999</v>
+      </c>
+      <c r="S13">
+        <v>0.31988800000000001</v>
+      </c>
+      <c r="T13">
+        <v>0.92479199999999995</v>
+      </c>
+      <c r="U13">
+        <v>0.83425099999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14">
+        <v>8192</v>
+      </c>
+      <c r="C14">
+        <v>16</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14" t="s">
+        <v>77</v>
+      </c>
+      <c r="H14">
+        <v>10</v>
+      </c>
+      <c r="I14">
+        <v>10</v>
+      </c>
+      <c r="J14">
+        <v>70</v>
+      </c>
+      <c r="K14">
+        <v>0.709144</v>
+      </c>
+      <c r="L14">
+        <v>0.97078600000000004</v>
+      </c>
+      <c r="M14">
+        <v>0.97384400000000004</v>
+      </c>
+      <c r="N14">
+        <v>0.96157199999999998</v>
+      </c>
+      <c r="O14">
+        <v>0.72860000000000003</v>
+      </c>
+      <c r="P14">
+        <v>0.56199900000000003</v>
+      </c>
+      <c r="Q14">
+        <v>0.52822400000000003</v>
+      </c>
+      <c r="R14">
+        <v>0.51474299999999995</v>
+      </c>
+      <c r="S14">
+        <v>0.32421499999999998</v>
+      </c>
+      <c r="T14">
+        <v>0.93037400000000003</v>
+      </c>
+      <c r="U14">
+        <v>0.85872599999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15">
+        <v>8192</v>
+      </c>
+      <c r="C15">
+        <v>16</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15" t="s">
+        <v>78</v>
+      </c>
+      <c r="H15">
+        <v>10</v>
+      </c>
+      <c r="I15">
         <v>10</v>
       </c>
     </row>
@@ -2702,15 +2976,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.125" customWidth="1"/>
+    <col min="1" max="1" width="19.5" customWidth="1"/>
     <col min="2" max="2" width="15.25" customWidth="1"/>
     <col min="3" max="3" width="9.875" customWidth="1"/>
   </cols>
@@ -3003,6 +3277,70 @@
         <v>0.78215082688839299</v>
       </c>
     </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10">
+        <v>21</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.70738430361082705</v>
+      </c>
+      <c r="E10">
+        <v>0.93276490158814795</v>
+      </c>
+      <c r="F10">
+        <v>0.93078706625653496</v>
+      </c>
+      <c r="G10">
+        <v>0.53751448906414101</v>
+      </c>
+      <c r="H10">
+        <v>0.93592079375042803</v>
+      </c>
+      <c r="I10">
+        <v>0.31871979918418503</v>
+      </c>
+      <c r="J10">
+        <v>0.813979369798847</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11">
+        <v>20</v>
+      </c>
+      <c r="D11">
+        <v>0.66276731924896803</v>
+      </c>
+      <c r="E11">
+        <v>0.88658788900812502</v>
+      </c>
+      <c r="F11">
+        <v>0.84287136801335905</v>
+      </c>
+      <c r="G11">
+        <v>0.40826445458976102</v>
+      </c>
+      <c r="H11">
+        <v>0.92232613436927902</v>
+      </c>
+      <c r="I11">
+        <v>0.32239884632597898</v>
+      </c>
+      <c r="J11">
+        <v>0.81797579294646106</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
implement dgcnn for segmentation
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -10,6 +10,7 @@
     <sheet name="semantic3d" sheetId="1" r:id="rId1"/>
     <sheet name="npm3d" sheetId="2" r:id="rId2"/>
     <sheet name="common_class" sheetId="3" r:id="rId3"/>
+    <sheet name="convpoint" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="88">
   <si>
     <t>model_name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -328,6 +329,42 @@
   </si>
   <si>
     <t>[0:7](v3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>convpoint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[0:1](v3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>use_color</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>use_intensity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mIoU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>convpoint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[1:2](v3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgcnn</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2010,10 +2047,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U15"/>
+  <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2874,7 +2911,7 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B14">
@@ -2939,7 +2976,7 @@
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B15">
@@ -2964,6 +3001,230 @@
         <v>10</v>
       </c>
       <c r="I15">
+        <v>10</v>
+      </c>
+      <c r="J15">
+        <v>61</v>
+      </c>
+      <c r="K15">
+        <v>0.71947099999999997</v>
+      </c>
+      <c r="L15">
+        <v>0.97270800000000002</v>
+      </c>
+      <c r="M15">
+        <v>0.97625200000000001</v>
+      </c>
+      <c r="N15">
+        <v>0.96355299999999999</v>
+      </c>
+      <c r="O15">
+        <v>0.64958700000000003</v>
+      </c>
+      <c r="P15">
+        <v>0.62269799999999997</v>
+      </c>
+      <c r="Q15">
+        <v>0.60464399999999996</v>
+      </c>
+      <c r="R15">
+        <v>0.56358900000000001</v>
+      </c>
+      <c r="S15">
+        <v>0.29377999999999999</v>
+      </c>
+      <c r="T15">
+        <v>0.93228800000000001</v>
+      </c>
+      <c r="U15">
+        <v>0.86884799999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16">
+        <v>8192</v>
+      </c>
+      <c r="C16">
+        <v>24</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>10</v>
+      </c>
+      <c r="I16">
+        <v>10</v>
+      </c>
+      <c r="J16">
+        <v>70</v>
+      </c>
+      <c r="K16">
+        <v>0.69466000000000006</v>
+      </c>
+      <c r="L16">
+        <v>0.97370400000000001</v>
+      </c>
+      <c r="M16">
+        <v>0.98242300000000005</v>
+      </c>
+      <c r="N16">
+        <v>0.96644200000000002</v>
+      </c>
+      <c r="O16">
+        <v>0.67562800000000001</v>
+      </c>
+      <c r="P16">
+        <v>0.59367899999999996</v>
+      </c>
+      <c r="Q16">
+        <v>0.48457499999999998</v>
+      </c>
+      <c r="R16">
+        <v>0.54436499999999999</v>
+      </c>
+      <c r="S16">
+        <v>0.211067</v>
+      </c>
+      <c r="T16">
+        <v>0.93242199999999997</v>
+      </c>
+      <c r="U16">
+        <v>0.86133599999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <v>8192</v>
+      </c>
+      <c r="C17">
+        <v>16</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>80</v>
+      </c>
+      <c r="H17">
+        <v>10</v>
+      </c>
+      <c r="I17">
+        <v>10</v>
+      </c>
+      <c r="J17">
+        <v>205</v>
+      </c>
+      <c r="K17">
+        <v>0.70485200000000003</v>
+      </c>
+      <c r="L17">
+        <v>0.96953299999999998</v>
+      </c>
+      <c r="M17">
+        <v>0.97586700000000004</v>
+      </c>
+      <c r="N17">
+        <v>0.95692999999999995</v>
+      </c>
+      <c r="O17">
+        <v>0.72497999999999996</v>
+      </c>
+      <c r="P17">
+        <v>0.60528999999999999</v>
+      </c>
+      <c r="Q17">
+        <v>0.54253799999999996</v>
+      </c>
+      <c r="R17">
+        <v>0.54025199999999995</v>
+      </c>
+      <c r="S17">
+        <v>0.26972299999999999</v>
+      </c>
+      <c r="T17">
+        <v>0.88974500000000001</v>
+      </c>
+      <c r="U17">
+        <v>0.83834299999999995</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>8192</v>
+      </c>
+      <c r="C18">
+        <v>16</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18" t="s">
+        <v>86</v>
+      </c>
+      <c r="H18">
+        <v>10</v>
+      </c>
+      <c r="I18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19">
+        <v>8192</v>
+      </c>
+      <c r="C19">
+        <v>8</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>10</v>
+      </c>
+      <c r="I19">
         <v>10</v>
       </c>
     </row>
@@ -2979,7 +3240,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3346,4 +3607,102 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.75" customWidth="1"/>
+    <col min="2" max="2" width="11.75" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="12.125" customWidth="1"/>
+    <col min="5" max="5" width="13.375" customWidth="1"/>
+    <col min="7" max="7" width="11.375" customWidth="1"/>
+    <col min="8" max="8" width="12.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" t="s">
+        <v>83</v>
+      </c>
+      <c r="M1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2">
+        <v>8192</v>
+      </c>
+      <c r="C2">
+        <v>16</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>8</v>
+      </c>
+      <c r="J2">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
implement atlasnet and capsule net
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="95">
   <si>
     <t>model_name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -365,6 +365,34 @@
   </si>
   <si>
     <t>dgcnn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[2:3](v3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[3:4](v3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[4:5](v3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[5:6](v3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pointsemantic_cross(cross_util)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pointsemantic_cross(piontnet_util)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[6:7](v3)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -710,10 +738,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T21"/>
+  <dimension ref="A1:T26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="T26" sqref="T26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1977,7 +2005,7 @@
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B21">
@@ -2036,6 +2064,316 @@
       </c>
       <c r="T21">
         <v>0.62772845604432204</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22">
+        <v>8192</v>
+      </c>
+      <c r="C22">
+        <v>24</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>10</v>
+      </c>
+      <c r="I22">
+        <v>10</v>
+      </c>
+      <c r="J22">
+        <v>80</v>
+      </c>
+      <c r="K22">
+        <v>0.67271999999999998</v>
+      </c>
+      <c r="L22">
+        <v>0.89093999999999995</v>
+      </c>
+      <c r="M22">
+        <v>0.91526099999999999</v>
+      </c>
+      <c r="N22">
+        <v>0.74115299999999995</v>
+      </c>
+      <c r="O22">
+        <v>0.8599</v>
+      </c>
+      <c r="P22">
+        <v>0.35096899999999998</v>
+      </c>
+      <c r="Q22">
+        <v>0.904864</v>
+      </c>
+      <c r="R22">
+        <v>0.289746</v>
+      </c>
+      <c r="S22">
+        <v>0.62039800000000001</v>
+      </c>
+      <c r="T22">
+        <v>0.69946900000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23">
+        <v>8192</v>
+      </c>
+      <c r="C23">
+        <v>24</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>10</v>
+      </c>
+      <c r="I23">
+        <v>10</v>
+      </c>
+      <c r="J23">
+        <v>75</v>
+      </c>
+      <c r="K23">
+        <v>0.57532700000000003</v>
+      </c>
+      <c r="L23">
+        <v>0.85615799999999997</v>
+      </c>
+      <c r="M23">
+        <v>0.75716499999999998</v>
+      </c>
+      <c r="N23">
+        <v>0.28651900000000002</v>
+      </c>
+      <c r="O23">
+        <v>0.89260899999999999</v>
+      </c>
+      <c r="P23">
+        <v>0.39098899999999998</v>
+      </c>
+      <c r="Q23">
+        <v>0.88710699999999998</v>
+      </c>
+      <c r="R23">
+        <v>0.27506599999999998</v>
+      </c>
+      <c r="S23">
+        <v>0.54597399999999996</v>
+      </c>
+      <c r="T23">
+        <v>0.567187</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24">
+        <v>8192</v>
+      </c>
+      <c r="C24">
+        <v>8</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>10</v>
+      </c>
+      <c r="I24">
+        <v>10</v>
+      </c>
+      <c r="J24">
+        <v>55</v>
+      </c>
+      <c r="K24">
+        <v>0.50617100000000004</v>
+      </c>
+      <c r="L24">
+        <v>0.834704</v>
+      </c>
+      <c r="M24">
+        <v>0.76049800000000001</v>
+      </c>
+      <c r="N24">
+        <v>0.15958900000000001</v>
+      </c>
+      <c r="O24">
+        <v>0.85673900000000003</v>
+      </c>
+      <c r="P24">
+        <v>0.32217400000000002</v>
+      </c>
+      <c r="Q24">
+        <v>0.86804400000000004</v>
+      </c>
+      <c r="R24">
+        <v>0.22381999999999999</v>
+      </c>
+      <c r="S24">
+        <v>0.48061300000000001</v>
+      </c>
+      <c r="T24">
+        <v>0.37789499999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25">
+        <v>4096</v>
+      </c>
+      <c r="C25">
+        <v>12</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>10</v>
+      </c>
+      <c r="I25">
+        <v>10</v>
+      </c>
+      <c r="J25">
+        <v>50</v>
+      </c>
+      <c r="K25">
+        <v>0.58433000000000002</v>
+      </c>
+      <c r="L25">
+        <v>0.86779600000000001</v>
+      </c>
+      <c r="M25">
+        <v>0.75122699999999998</v>
+      </c>
+      <c r="N25">
+        <v>0.24152699999999999</v>
+      </c>
+      <c r="O25">
+        <v>0.90471299999999999</v>
+      </c>
+      <c r="P25">
+        <v>0.378224</v>
+      </c>
+      <c r="Q25">
+        <v>0.91183400000000003</v>
+      </c>
+      <c r="R25">
+        <v>0.37094700000000003</v>
+      </c>
+      <c r="S25">
+        <v>0.54784100000000002</v>
+      </c>
+      <c r="T25">
+        <v>0.56832400000000005</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B26">
+        <v>4096</v>
+      </c>
+      <c r="C26">
+        <v>12</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>10</v>
+      </c>
+      <c r="I26">
+        <v>10</v>
+      </c>
+      <c r="J26">
+        <v>80</v>
+      </c>
+      <c r="K26">
+        <v>0.56943200000000005</v>
+      </c>
+      <c r="L26">
+        <v>0.85506700000000002</v>
+      </c>
+      <c r="M26">
+        <v>0.75760499999999997</v>
+      </c>
+      <c r="N26">
+        <v>0.19888500000000001</v>
+      </c>
+      <c r="O26">
+        <v>0.89702000000000004</v>
+      </c>
+      <c r="P26">
+        <v>0.36307899999999999</v>
+      </c>
+      <c r="Q26">
+        <v>0.89568899999999996</v>
+      </c>
+      <c r="R26">
+        <v>0.30738300000000002</v>
+      </c>
+      <c r="S26">
+        <v>0.560419</v>
+      </c>
+      <c r="T26">
+        <v>0.57537700000000003</v>
       </c>
     </row>
   </sheetData>
@@ -2047,10 +2385,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U19"/>
+  <dimension ref="A1:U25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3041,7 +3379,7 @@
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>79</v>
       </c>
       <c r="B16">
@@ -3198,9 +3536,45 @@
       <c r="I18">
         <v>10</v>
       </c>
+      <c r="J18">
+        <v>115</v>
+      </c>
+      <c r="K18">
+        <v>0.68501599999999996</v>
+      </c>
+      <c r="L18">
+        <v>0.96877100000000005</v>
+      </c>
+      <c r="M18">
+        <v>0.97485900000000003</v>
+      </c>
+      <c r="N18">
+        <v>0.95752800000000005</v>
+      </c>
+      <c r="O18">
+        <v>0.70303400000000005</v>
+      </c>
+      <c r="P18">
+        <v>0.63248099999999996</v>
+      </c>
+      <c r="Q18">
+        <v>0.46900700000000001</v>
+      </c>
+      <c r="R18">
+        <v>0.49063499999999999</v>
+      </c>
+      <c r="S18">
+        <v>0.19828799999999999</v>
+      </c>
+      <c r="T18">
+        <v>0.90672399999999997</v>
+      </c>
+      <c r="U18">
+        <v>0.83258799999999999</v>
+      </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B19">
@@ -3225,6 +3599,396 @@
         <v>10</v>
       </c>
       <c r="I19">
+        <v>10</v>
+      </c>
+      <c r="J19">
+        <v>50</v>
+      </c>
+      <c r="K19">
+        <v>0.57953299999999996</v>
+      </c>
+      <c r="L19">
+        <v>0.94918800000000003</v>
+      </c>
+      <c r="M19">
+        <v>0.97648999999999997</v>
+      </c>
+      <c r="N19">
+        <v>0.93071300000000001</v>
+      </c>
+      <c r="O19">
+        <v>0.584152</v>
+      </c>
+      <c r="P19">
+        <v>0.42607899999999999</v>
+      </c>
+      <c r="Q19">
+        <v>0.23447899999999999</v>
+      </c>
+      <c r="R19">
+        <v>0.32186700000000001</v>
+      </c>
+      <c r="S19">
+        <v>0.20671999999999999</v>
+      </c>
+      <c r="T19">
+        <v>0.80191400000000002</v>
+      </c>
+      <c r="U19">
+        <v>0.73338599999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>8192</v>
+      </c>
+      <c r="C20">
+        <v>16</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20" t="s">
+        <v>88</v>
+      </c>
+      <c r="H20">
+        <v>10</v>
+      </c>
+      <c r="I20">
+        <v>10</v>
+      </c>
+      <c r="J20">
+        <v>70</v>
+      </c>
+      <c r="K20">
+        <v>0.70216299999999998</v>
+      </c>
+      <c r="L20">
+        <v>0.96774400000000005</v>
+      </c>
+      <c r="M20">
+        <v>0.97522299999999995</v>
+      </c>
+      <c r="N20">
+        <v>0.95728800000000003</v>
+      </c>
+      <c r="O20">
+        <v>0.65977399999999997</v>
+      </c>
+      <c r="P20">
+        <v>0.59978200000000004</v>
+      </c>
+      <c r="Q20">
+        <v>0.451096</v>
+      </c>
+      <c r="R20">
+        <v>0.51560499999999998</v>
+      </c>
+      <c r="S20">
+        <v>0.430728</v>
+      </c>
+      <c r="T20">
+        <v>0.90354999999999996</v>
+      </c>
+      <c r="U20">
+        <v>0.82641900000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>8192</v>
+      </c>
+      <c r="C21">
+        <v>16</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21" t="s">
+        <v>89</v>
+      </c>
+      <c r="H21">
+        <v>10</v>
+      </c>
+      <c r="I21">
+        <v>10</v>
+      </c>
+      <c r="J21">
+        <v>50</v>
+      </c>
+      <c r="K21">
+        <v>0.67153799999999997</v>
+      </c>
+      <c r="L21">
+        <v>0.96775800000000001</v>
+      </c>
+      <c r="M21">
+        <v>0.976051</v>
+      </c>
+      <c r="N21">
+        <v>0.95656699999999995</v>
+      </c>
+      <c r="O21">
+        <v>0.66411600000000004</v>
+      </c>
+      <c r="P21">
+        <v>0.57963600000000004</v>
+      </c>
+      <c r="Q21">
+        <v>0.427954</v>
+      </c>
+      <c r="R21">
+        <v>0.498033</v>
+      </c>
+      <c r="S21">
+        <v>0.211982</v>
+      </c>
+      <c r="T21">
+        <v>0.90212400000000004</v>
+      </c>
+      <c r="U21">
+        <v>0.82738199999999995</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>8192</v>
+      </c>
+      <c r="C22">
+        <v>16</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22" t="s">
+        <v>90</v>
+      </c>
+      <c r="H22">
+        <v>10</v>
+      </c>
+      <c r="I22">
+        <v>10</v>
+      </c>
+      <c r="J22">
+        <v>40</v>
+      </c>
+      <c r="K22">
+        <v>0.68883000000000005</v>
+      </c>
+      <c r="L22">
+        <v>0.96425700000000003</v>
+      </c>
+      <c r="M22">
+        <v>0.97096300000000002</v>
+      </c>
+      <c r="N22">
+        <v>0.95480600000000004</v>
+      </c>
+      <c r="O22">
+        <v>0.64660899999999999</v>
+      </c>
+      <c r="P22">
+        <v>0.59869899999999998</v>
+      </c>
+      <c r="Q22">
+        <v>0.50395199999999996</v>
+      </c>
+      <c r="R22">
+        <v>0.52042999999999995</v>
+      </c>
+      <c r="S22">
+        <v>0.34489300000000001</v>
+      </c>
+      <c r="T22">
+        <v>0.87926199999999999</v>
+      </c>
+      <c r="U22">
+        <v>0.77989560000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23">
+        <v>8192</v>
+      </c>
+      <c r="C23">
+        <v>16</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23" t="s">
+        <v>91</v>
+      </c>
+      <c r="H23">
+        <v>10</v>
+      </c>
+      <c r="I23">
+        <v>10</v>
+      </c>
+      <c r="J23">
+        <v>105</v>
+      </c>
+      <c r="K23">
+        <v>0.72541599999999995</v>
+      </c>
+      <c r="L23">
+        <v>0.96925600000000001</v>
+      </c>
+      <c r="M23">
+        <v>0.97574000000000005</v>
+      </c>
+      <c r="N23">
+        <v>0.96232399999999996</v>
+      </c>
+      <c r="O23">
+        <v>0.67620899999999995</v>
+      </c>
+      <c r="P23">
+        <v>0.63898600000000005</v>
+      </c>
+      <c r="Q23">
+        <v>0.48246800000000001</v>
+      </c>
+      <c r="R23">
+        <v>0.52152900000000002</v>
+      </c>
+      <c r="S23">
+        <v>0.55739300000000003</v>
+      </c>
+      <c r="T23">
+        <v>0.89163599999999998</v>
+      </c>
+      <c r="U23">
+        <v>0.82245500000000005</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24">
+        <v>8192</v>
+      </c>
+      <c r="C24">
+        <v>16</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24" t="s">
+        <v>94</v>
+      </c>
+      <c r="H24">
+        <v>10</v>
+      </c>
+      <c r="I24">
+        <v>10</v>
+      </c>
+      <c r="J24">
+        <v>85</v>
+      </c>
+      <c r="K24">
+        <v>0.68441300000000005</v>
+      </c>
+      <c r="L24">
+        <v>0.96577900000000005</v>
+      </c>
+      <c r="M24">
+        <v>0.97875900000000005</v>
+      </c>
+      <c r="N24">
+        <v>0.95107299999999995</v>
+      </c>
+      <c r="O24">
+        <v>0.67345100000000002</v>
+      </c>
+      <c r="P24">
+        <v>0.63883900000000005</v>
+      </c>
+      <c r="Q24">
+        <v>0.45552399999999998</v>
+      </c>
+      <c r="R24">
+        <v>0.45928999999999998</v>
+      </c>
+      <c r="S24">
+        <v>0.26414700000000002</v>
+      </c>
+      <c r="T24">
+        <v>0.90571800000000002</v>
+      </c>
+      <c r="U24">
+        <v>0.83291199999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25">
+        <v>8192</v>
+      </c>
+      <c r="C25">
+        <v>16</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25" t="s">
+        <v>94</v>
+      </c>
+      <c r="H25">
+        <v>10</v>
+      </c>
+      <c r="I25">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add geometry v3 to semantic_dataset.py
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="semantic3d" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="97">
   <si>
     <t>model_name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -397,6 +397,10 @@
   </si>
   <si>
     <t>pointsemantic_cross(pointnet_util)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pointsemantic(cross_util)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -742,15 +746,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T26"/>
+  <dimension ref="A1:T27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.5" customWidth="1"/>
+    <col min="1" max="1" width="30.875" customWidth="1"/>
     <col min="2" max="2" width="11.875" customWidth="1"/>
     <col min="3" max="3" width="10.625" customWidth="1"/>
     <col min="4" max="4" width="11.875" customWidth="1"/>
@@ -2380,6 +2384,35 @@
         <v>0.57537700000000003</v>
       </c>
     </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27">
+        <v>8192</v>
+      </c>
+      <c r="C27">
+        <v>16</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>10</v>
+      </c>
+      <c r="I27">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2389,10 +2422,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U26"/>
+  <dimension ref="A1:U27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4060,6 +4093,107 @@
       <c r="I26">
         <v>10</v>
       </c>
+      <c r="J26">
+        <v>60</v>
+      </c>
+      <c r="K26">
+        <v>0.66763099999999997</v>
+      </c>
+      <c r="L26">
+        <v>0.96370800000000001</v>
+      </c>
+      <c r="M26">
+        <v>0.97444299999999995</v>
+      </c>
+      <c r="N26">
+        <v>0.95304299999999997</v>
+      </c>
+      <c r="O26">
+        <v>0.68271499999999996</v>
+      </c>
+      <c r="P26">
+        <v>0.62173400000000001</v>
+      </c>
+      <c r="Q26">
+        <v>0.42114099999999999</v>
+      </c>
+      <c r="R26">
+        <v>0.429734</v>
+      </c>
+      <c r="S26">
+        <v>0.27828999999999998</v>
+      </c>
+      <c r="T26">
+        <v>0.85603200000000002</v>
+      </c>
+      <c r="U26">
+        <v>0.79154400000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27">
+        <v>8192</v>
+      </c>
+      <c r="C27">
+        <v>16</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>10</v>
+      </c>
+      <c r="I27">
+        <v>10</v>
+      </c>
+      <c r="J27">
+        <v>110</v>
+      </c>
+      <c r="K27">
+        <v>0.71029699999999996</v>
+      </c>
+      <c r="L27">
+        <v>0.96879400000000004</v>
+      </c>
+      <c r="M27">
+        <v>0.97430799999999995</v>
+      </c>
+      <c r="N27">
+        <v>0.957426</v>
+      </c>
+      <c r="O27">
+        <v>0.67928200000000005</v>
+      </c>
+      <c r="P27">
+        <v>0.64705900000000005</v>
+      </c>
+      <c r="Q27">
+        <v>0.44625399999999998</v>
+      </c>
+      <c r="R27">
+        <v>0.51074699999999995</v>
+      </c>
+      <c r="S27">
+        <v>0.42068</v>
+      </c>
+      <c r="T27">
+        <v>0.922037</v>
+      </c>
+      <c r="U27">
+        <v>0.83487800000000001</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -4073,7 +4207,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4447,7 +4581,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>